<commit_message>
Second commit for code modifications.
</commit_message>
<xml_diff>
--- a/cypress/downloads/All_data_01.02.2024_-_29.02.2024.xlsx
+++ b/cypress/downloads/All_data_01.02.2024_-_29.02.2024.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="69" xml:space="preserve">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="71" xml:space="preserve">
   <si>
     <t>Casio2 GmbH Test</t>
   </si>
@@ -77,7 +77,7 @@
     <t>01:10</t>
   </si>
   <si>
-    <t>11:01</t>
+    <t>14:07</t>
   </si>
   <si>
     <t>Project A</t>
@@ -198,6 +198,12 @@
   </si>
   <si>
     <t>07:32</t>
+  </si>
+  <si>
+    <t>11:01</t>
+  </si>
+  <si>
+    <t>14:06</t>
   </si>
   <si>
     <t>Start Date</t>
@@ -1108,7 +1114,7 @@
         <v>5</v>
       </c>
       <c r="N4" s="9" t="n">
-        <v>-17621.1075</v>
+        <v>-17621.105277777777</v>
       </c>
       <c r="O4" s="9"/>
       <c r="P4" s="9"/>
@@ -1176,23 +1182,23 @@
         <v>21</v>
       </c>
       <c r="G6" s="14" t="n">
-        <v>0.02</v>
+        <v>0.02611111111111111</v>
       </c>
       <c r="H6" s="14" t="n">
-        <v>3.4786111111111113</v>
+        <v>3.4808333333333334</v>
       </c>
       <c r="I6" s="14" t="n">
         <v>0.0</v>
       </c>
       <c r="J6" s="24"/>
       <c r="K6" s="14" t="n">
-        <v>3.4786111111111113</v>
+        <v>3.4808333333333334</v>
       </c>
       <c r="L6" s="14" t="n">
         <v>1.0</v>
       </c>
       <c r="M6" s="14" t="n">
-        <v>2.4786111111111113</v>
+        <v>2.4808333333333334</v>
       </c>
       <c r="N6" s="22" t="inlineStr">
         <is>
@@ -21256,7 +21262,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L16"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView windowProtection="0" tabSelected="0" showWhiteSpace="0" showOutlineSymbols="0" showFormulas="0" rightToLeft="0" showZeros="1" showRuler="1" showRowColHeaders="1" showGridLines="1" defaultGridColor="1" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
@@ -21622,7 +21628,7 @@
         <v>45323.0</v>
       </c>
       <c r="E11" s="41" t="s">
-        <v>20</v>
+        <v>61</v>
       </c>
       <c r="F11" s="36" t="s">
         <v>21</v>
@@ -21649,136 +21655,216 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="34" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="42">
+      <c r="A12" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="43">
         <v>45323.0</v>
       </c>
-      <c r="C12" s="40" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="42">
+      <c r="C12" s="41" t="s">
+        <v>62</v>
+      </c>
+      <c r="D12" s="43">
         <v>45323.0</v>
       </c>
-      <c r="E12" s="40" t="s">
-        <v>23</v>
-      </c>
-      <c r="F12" s="34" t="inlineStr">
+      <c r="E12" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" s="36" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="G12" s="34" t="inlineStr">
+      <c r="H12" s="37" t="n">
+        <v>0.005833333333333333</v>
+      </c>
+      <c r="I12" s="37" t="n">
+        <v>0.0005555555555555556</v>
+      </c>
+      <c r="J12" s="37" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K12" s="48"/>
+      <c r="L12" s="46" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="H12" s="35" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="I12" s="35" t="n">
-        <v>0.0005555555555555556</v>
-      </c>
-      <c r="J12" s="35" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="K12" s="47"/>
-      <c r="L12" s="45" t="inlineStr">
+    </row>
+    <row r="13">
+      <c r="A13" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="43">
+        <v>45323.0</v>
+      </c>
+      <c r="C13" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="43">
+        <v>45323.0</v>
+      </c>
+      <c r="E13" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" s="36" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="38" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="42">
-        <v>45323.0</v>
-      </c>
-      <c r="C13" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="42">
-        <v>45323.0</v>
-      </c>
-      <c r="E13" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="F13" s="34" t="inlineStr">
+      <c r="H13" s="37" t="n">
+        <v>0.0002777777777777778</v>
+      </c>
+      <c r="I13" s="37" t="n">
+        <v>0.0016666666666666668</v>
+      </c>
+      <c r="J13" s="37" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K13" s="48"/>
+      <c r="L13" s="46" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="G13" s="34" t="inlineStr">
+    </row>
+    <row r="14">
+      <c r="A14" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="42">
+        <v>45323.0</v>
+      </c>
+      <c r="C14" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="42">
+        <v>45323.0</v>
+      </c>
+      <c r="E14" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" s="34" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="H13" s="35" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="I13" s="35" t="n">
-        <v>0.0019444444444444444</v>
-      </c>
-      <c r="J13" s="35" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="K13" s="47"/>
-      <c r="L13" s="45" t="inlineStr">
+      <c r="G14" s="34" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="44"/>
-      <c r="B14" s="44"/>
-      <c r="C14" s="44"/>
-      <c r="D14" s="44"/>
-      <c r="E14" s="44"/>
-      <c r="F14" s="44"/>
-      <c r="G14" s="44"/>
-      <c r="H14" s="44" t="str">
-        <f>SUM(H5:H13)</f>
-      </c>
-      <c r="I14" s="44" t="str">
-        <f>SUM(I5:I13)</f>
-      </c>
-      <c r="J14" s="44" t="str">
-        <f>SUM(J5:J13)</f>
-      </c>
-      <c r="K14" s="44"/>
-      <c r="L14" s="44"/>
+      <c r="H14" s="35" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I14" s="35" t="n">
+        <v>0.0005555555555555556</v>
+      </c>
+      <c r="J14" s="35" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K14" s="47"/>
+      <c r="L14" s="45" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
     </row>
     <row r="15">
-      <c r="A15" s="49"/>
-      <c r="B15" s="49"/>
-      <c r="C15" s="49"/>
-      <c r="D15" s="49"/>
-      <c r="E15" s="49"/>
-      <c r="F15" s="49"/>
-      <c r="G15" s="49"/>
-      <c r="H15" s="49"/>
-      <c r="I15" s="49"/>
-      <c r="J15" s="49"/>
-      <c r="K15" s="49"/>
-      <c r="L15" s="49"/>
+      <c r="A15" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="42">
+        <v>45323.0</v>
+      </c>
+      <c r="C15" s="40" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="42">
+        <v>45323.0</v>
+      </c>
+      <c r="E15" s="40" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15" s="34" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="G15" s="34" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H15" s="35" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I15" s="35" t="n">
+        <v>0.0019444444444444444</v>
+      </c>
+      <c r="J15" s="35" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K15" s="47"/>
+      <c r="L15" s="45" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
     </row>
     <row r="16">
-      <c r="A16" s="49"/>
-      <c r="B16" s="49"/>
-      <c r="C16" s="49"/>
-      <c r="D16" s="49"/>
-      <c r="E16" s="49"/>
-      <c r="F16" s="49"/>
-      <c r="G16" s="49"/>
-      <c r="H16" s="49"/>
-      <c r="I16" s="49"/>
-      <c r="J16" s="49"/>
-      <c r="K16" s="49"/>
-      <c r="L16" s="49" t="s">
+      <c r="A16" s="44"/>
+      <c r="B16" s="44"/>
+      <c r="C16" s="44"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="44"/>
+      <c r="F16" s="44"/>
+      <c r="G16" s="44"/>
+      <c r="H16" s="44" t="str">
+        <f>SUM(H5:H15)</f>
+      </c>
+      <c r="I16" s="44" t="str">
+        <f>SUM(I5:I15)</f>
+      </c>
+      <c r="J16" s="44" t="str">
+        <f>SUM(J5:J15)</f>
+      </c>
+      <c r="K16" s="44"/>
+      <c r="L16" s="44"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="49"/>
+      <c r="B17" s="49"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="49"/>
+      <c r="F17" s="49"/>
+      <c r="G17" s="49"/>
+      <c r="H17" s="49"/>
+      <c r="I17" s="49"/>
+      <c r="J17" s="49"/>
+      <c r="K17" s="49"/>
+      <c r="L17" s="49"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="49"/>
+      <c r="B18" s="49"/>
+      <c r="C18" s="49"/>
+      <c r="D18" s="49"/>
+      <c r="E18" s="49"/>
+      <c r="F18" s="49"/>
+      <c r="G18" s="49"/>
+      <c r="H18" s="49"/>
+      <c r="I18" s="49"/>
+      <c r="J18" s="49"/>
+      <c r="K18" s="49"/>
+      <c r="L18" s="49" t="s">
         <v>51</v>
       </c>
     </row>
@@ -21804,7 +21890,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:P10"/>
+  <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView windowProtection="0" tabSelected="0" showWhiteSpace="0" showOutlineSymbols="0" showFormulas="0" rightToLeft="0" showZeros="1" showRuler="1" showRowColHeaders="1" showGridLines="1" defaultGridColor="1" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
@@ -21833,16 +21919,16 @@
         <v>6</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="F1" s="0" t="s">
         <v>53</v>
@@ -21866,16 +21952,16 @@
         <v>17</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2">
@@ -22156,7 +22242,7 @@
         <v>45323.0</v>
       </c>
       <c r="E8" s="50" t="s">
-        <v>20</v>
+        <v>61</v>
       </c>
       <c r="F8" s="0" t="s">
         <v>21</v>
@@ -22188,24 +22274,22 @@
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B9" s="2">
         <v>45323.0</v>
       </c>
       <c r="C9" s="50" t="s">
-        <v>23</v>
+        <v>62</v>
       </c>
       <c r="D9" s="2">
         <v>45323.0</v>
       </c>
       <c r="E9" s="50" t="s">
-        <v>23</v>
-      </c>
-      <c r="F9" s="0" t="inlineStr">
-        <is>
-          <t/>
-        </is>
+        <v>20</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>21</v>
       </c>
       <c r="G9" s="0" t="inlineStr">
         <is>
@@ -22213,7 +22297,7 @@
         </is>
       </c>
       <c r="H9" s="51" t="n">
-        <v>0.0</v>
+        <v>0.00024305555555555552</v>
       </c>
       <c r="I9" s="51" t="n">
         <v>2.3148148148148147e-05</v>
@@ -22234,24 +22318,22 @@
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B10" s="2">
         <v>45323.0</v>
       </c>
       <c r="C10" s="50" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D10" s="2">
         <v>45323.0</v>
       </c>
       <c r="E10" s="50" t="s">
-        <v>24</v>
-      </c>
-      <c r="F10" s="0" t="inlineStr">
-        <is>
-          <t/>
-        </is>
+        <v>20</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>21</v>
       </c>
       <c r="G10" s="0" t="inlineStr">
         <is>
@@ -22259,10 +22341,10 @@
         </is>
       </c>
       <c r="H10" s="51" t="n">
-        <v>0.0</v>
+        <v>1.1574074074074073e-05</v>
       </c>
       <c r="I10" s="51" t="n">
-        <v>8.101851851851852e-05</v>
+        <v>6.944444444444444e-05</v>
       </c>
       <c r="J10" s="51" t="n">
         <v>0.0</v>
@@ -22277,6 +22359,98 @@
       <c r="N10" s="0"/>
       <c r="O10" s="0"/>
       <c r="P10" s="0"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="2">
+        <v>45323.0</v>
+      </c>
+      <c r="C11" s="50" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="2">
+        <v>45323.0</v>
+      </c>
+      <c r="E11" s="50" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="G11" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H11" s="51" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I11" s="51" t="n">
+        <v>2.3148148148148147e-05</v>
+      </c>
+      <c r="J11" s="51" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K11" s="0"/>
+      <c r="L11" s="52" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="M11" s="0"/>
+      <c r="N11" s="0"/>
+      <c r="O11" s="0"/>
+      <c r="P11" s="0"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="2">
+        <v>45323.0</v>
+      </c>
+      <c r="C12" s="50" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="2">
+        <v>45323.0</v>
+      </c>
+      <c r="E12" s="50" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="G12" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H12" s="51" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I12" s="51" t="n">
+        <v>8.101851851851852e-05</v>
+      </c>
+      <c r="J12" s="51" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K12" s="0"/>
+      <c r="L12" s="52" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="M12" s="0"/>
+      <c r="N12" s="0"/>
+      <c r="O12" s="0"/>
+      <c r="P12" s="0"/>
     </row>
   </sheetData>
   <sheetCalcPr fullCalcOnLoad="1"/>

</xml_diff>